<commit_message>
add Nano THC name
</commit_message>
<xml_diff>
--- a/database/MIT_database.xlsx
+++ b/database/MIT_database.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="FEA" sheetId="1" r:id="rId1"/>
-    <sheet name="History" sheetId="2" r:id="rId2"/>
+    <sheet name="History__" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="128">
   <si>
     <t>RunID</t>
   </si>
@@ -74,34 +74,196 @@
     <t>Belt displacement TS</t>
   </si>
   <si>
+    <t>Lap bracket force</t>
+  </si>
+  <si>
+    <t>HA torque</t>
+  </si>
+  <si>
+    <t>Backrest x displ</t>
+  </si>
+  <si>
+    <t>PELVIS DX</t>
+  </si>
+  <si>
+    <t>PELVIS DZ</t>
+  </si>
+  <si>
+    <t>Tilt Axial Force</t>
+  </si>
+  <si>
+    <t>Tilt Shear Force</t>
+  </si>
+  <si>
+    <t>Track sliding DS</t>
+  </si>
+  <si>
+    <t>Track sliding TS</t>
+  </si>
+  <si>
+    <t>Pinion torque</t>
+  </si>
+  <si>
+    <t>Res_F C_ROLLER_1-C_CAM</t>
+  </si>
+  <si>
+    <t>Res_F C_ROLLER_2-C_CAM</t>
+  </si>
+  <si>
+    <t>Res_F C_ROLLER_3-C_CAM</t>
+  </si>
+  <si>
+    <t>Res_F C_ROLLER_4-C_CAM</t>
+  </si>
+  <si>
+    <t>Res_F C_ROLLER_5-C_CAM</t>
+  </si>
+  <si>
+    <t>Res_F C_ROLLER_6-C_CAM</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_10-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_9-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_8-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_7-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_6-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_5-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_4-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_3-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_2-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_1-PINION</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_6-L_RING</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_5-L_RING</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_4-L_RING</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_3-L_RING</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_2-L_RING</t>
+  </si>
+  <si>
+    <t>Res_F L_ROLLER_1-L_RING</t>
+  </si>
+  <si>
+    <t>Res_F Pinion-Collar-1</t>
+  </si>
+  <si>
+    <t>Res_F Pinion-Collar-2</t>
+  </si>
+  <si>
+    <t>Torque MX on pinions section</t>
+  </si>
+  <si>
+    <t>Res Force C_ROLLER_1-C_CAM</t>
+  </si>
+  <si>
+    <t>Res Force C_ROLLER_2-C_CAM</t>
+  </si>
+  <si>
+    <t>Res Force C_ROLLER_3-C_CAM</t>
+  </si>
+  <si>
+    <t>Res Force C_ROLLER_4-C_CAM</t>
+  </si>
+  <si>
+    <t>Res Force C_ROLLER_5-C_CAM</t>
+  </si>
+  <si>
+    <t>Res Force C_ROLLER_6-C_CAM</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_10-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_9-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_8-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_7-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_6-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_5-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_4-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_3-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_2-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_1-PINION</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_6-L_RING</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_5-L_RING</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_4-L_RING</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_3-L_RING</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_2-L_RING</t>
+  </si>
+  <si>
+    <t>Res Force L_ROLLER_1-L_RING</t>
+  </si>
+  <si>
+    <t>Res Force Pinion-Collar-1</t>
+  </si>
+  <si>
+    <t>Res Force Pinion-Collar-2</t>
+  </si>
+  <si>
     <t>Rear bracket force DS</t>
   </si>
   <si>
-    <t>Lap bracket force</t>
-  </si>
-  <si>
-    <t>HA torque</t>
-  </si>
-  <si>
-    <t>Backrest x displ</t>
-  </si>
-  <si>
-    <t>PELVIS DX</t>
-  </si>
-  <si>
-    <t>PELVIS DZ</t>
-  </si>
-  <si>
-    <t>Tilt Axial Force</t>
-  </si>
-  <si>
-    <t>Tilt Shear Force</t>
-  </si>
-  <si>
-    <t>Track sliding DS</t>
-  </si>
-  <si>
-    <t>Track sliding TS</t>
+    <t>GR1912450</t>
+  </si>
+  <si>
+    <t>GR2013229</t>
+  </si>
+  <si>
+    <t>GR201398</t>
+  </si>
+  <si>
+    <t>GR206436</t>
   </si>
   <si>
     <t>GR206929</t>
@@ -113,54 +275,102 @@
     <t>GR207090</t>
   </si>
   <si>
+    <t>PSA</t>
+  </si>
+  <si>
     <t>VOLVO</t>
   </si>
   <si>
+    <t xml:space="preserve"> P2D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C4</t>
+  </si>
+  <si>
     <t xml:space="preserve"> SPA2-F</t>
   </si>
   <si>
+    <t>4WM</t>
+  </si>
+  <si>
+    <t>10WP</t>
+  </si>
+  <si>
     <t>8WP</t>
   </si>
   <si>
     <t>8WPP</t>
   </si>
   <si>
+    <t>Luggage crash</t>
+  </si>
+  <si>
     <t>Front Crash</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve"> D95</t>
   </si>
   <si>
     <t xml:space="preserve"> D50</t>
   </si>
   <si>
+    <t>DFNuC-F</t>
+  </si>
+  <si>
+    <t>DFNuC</t>
+  </si>
+  <si>
+    <t>F05</t>
+  </si>
+  <si>
     <t>K04-0</t>
   </si>
   <si>
+    <t>Tracks:rear most - 1 notch</t>
+  </si>
+  <si>
+    <t>Tracks:middle</t>
+  </si>
+  <si>
     <t>Tracks:rear most</t>
   </si>
   <si>
-    <t>Tracks:middle</t>
-  </si>
-  <si>
     <t xml:space="preserve"> HA:lower most</t>
   </si>
   <si>
     <t xml:space="preserve"> HA:middle</t>
   </si>
   <si>
+    <t xml:space="preserve"> Luggage-010</t>
+  </si>
+  <si>
     <t xml:space="preserve"> EuroNCAP40mph</t>
   </si>
   <si>
+    <t>OK Limit</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
     <t>NOK</t>
   </si>
   <si>
-    <t>OK Limit</t>
+    <t>None</t>
   </si>
   <si>
     <t>NOK Limit</t>
   </si>
   <si>
+    <t>LUG_ Rm-1nDm</t>
+  </si>
+  <si>
+    <t>FC95 MpDm</t>
+  </si>
+  <si>
     <t>FC95 RmDm</t>
   </si>
   <si>
@@ -179,7 +389,16 @@
     <t>07-01-2021 13:58:58</t>
   </si>
   <si>
+    <t>07-01-2021 14:54:07</t>
+  </si>
+  <si>
+    <t>07-01-2021 14:55:50</t>
+  </si>
+  <si>
     <t>GR206929,GR207006,GR207090</t>
+  </si>
+  <si>
+    <t>GR1912450,GR2013229,GR201398,GR206436</t>
   </si>
 </sst>
 </file>
@@ -227,9 +446,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FEA" displayName="FEA" ref="A1:AC4" totalsRowShown="0">
-  <autoFilter ref="A1:AC4"/>
-  <tableColumns count="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FEA" displayName="FEA" ref="A1:CA8" totalsRowShown="0">
+  <autoFilter ref="A1:CA8"/>
+  <tableColumns count="79">
     <tableColumn id="1" name="RunID"/>
     <tableColumn id="2" name="OEM"/>
     <tableColumn id="3" name="project_name"/>
@@ -249,24 +468,74 @@
     <tableColumn id="17" name="Recliner torque TS"/>
     <tableColumn id="18" name="Belt displacement DS"/>
     <tableColumn id="19" name="Belt displacement TS"/>
-    <tableColumn id="20" name="Rear bracket force DS"/>
-    <tableColumn id="21" name="Lap bracket force"/>
-    <tableColumn id="22" name="HA torque"/>
-    <tableColumn id="23" name="Backrest x displ"/>
-    <tableColumn id="24" name="PELVIS DX"/>
-    <tableColumn id="25" name="PELVIS DZ"/>
-    <tableColumn id="26" name="Tilt Axial Force"/>
-    <tableColumn id="27" name="Tilt Shear Force"/>
-    <tableColumn id="28" name="Track sliding DS"/>
-    <tableColumn id="29" name="Track sliding TS"/>
+    <tableColumn id="20" name="Lap bracket force"/>
+    <tableColumn id="21" name="HA torque"/>
+    <tableColumn id="22" name="Backrest x displ"/>
+    <tableColumn id="23" name="PELVIS DX"/>
+    <tableColumn id="24" name="PELVIS DZ"/>
+    <tableColumn id="25" name="Tilt Axial Force"/>
+    <tableColumn id="26" name="Tilt Shear Force"/>
+    <tableColumn id="27" name="Track sliding DS"/>
+    <tableColumn id="28" name="Track sliding TS"/>
+    <tableColumn id="29" name="Pinion torque"/>
+    <tableColumn id="30" name="Res_F C_ROLLER_1-C_CAM"/>
+    <tableColumn id="31" name="Res_F C_ROLLER_2-C_CAM"/>
+    <tableColumn id="32" name="Res_F C_ROLLER_3-C_CAM"/>
+    <tableColumn id="33" name="Res_F C_ROLLER_4-C_CAM"/>
+    <tableColumn id="34" name="Res_F C_ROLLER_5-C_CAM"/>
+    <tableColumn id="35" name="Res_F C_ROLLER_6-C_CAM"/>
+    <tableColumn id="36" name="Res_F L_ROLLER_10-PINION"/>
+    <tableColumn id="37" name="Res_F L_ROLLER_9-PINION"/>
+    <tableColumn id="38" name="Res_F L_ROLLER_8-PINION"/>
+    <tableColumn id="39" name="Res_F L_ROLLER_7-PINION"/>
+    <tableColumn id="40" name="Res_F L_ROLLER_6-PINION"/>
+    <tableColumn id="41" name="Res_F L_ROLLER_5-PINION"/>
+    <tableColumn id="42" name="Res_F L_ROLLER_4-PINION"/>
+    <tableColumn id="43" name="Res_F L_ROLLER_3-PINION"/>
+    <tableColumn id="44" name="Res_F L_ROLLER_2-PINION"/>
+    <tableColumn id="45" name="Res_F L_ROLLER_1-PINION"/>
+    <tableColumn id="46" name="Res_F L_ROLLER_6-L_RING"/>
+    <tableColumn id="47" name="Res_F L_ROLLER_5-L_RING"/>
+    <tableColumn id="48" name="Res_F L_ROLLER_4-L_RING"/>
+    <tableColumn id="49" name="Res_F L_ROLLER_3-L_RING"/>
+    <tableColumn id="50" name="Res_F L_ROLLER_2-L_RING"/>
+    <tableColumn id="51" name="Res_F L_ROLLER_1-L_RING"/>
+    <tableColumn id="52" name="Res_F Pinion-Collar-1"/>
+    <tableColumn id="53" name="Res_F Pinion-Collar-2"/>
+    <tableColumn id="54" name="Torque MX on pinions section"/>
+    <tableColumn id="55" name="Res Force C_ROLLER_1-C_CAM"/>
+    <tableColumn id="56" name="Res Force C_ROLLER_2-C_CAM"/>
+    <tableColumn id="57" name="Res Force C_ROLLER_3-C_CAM"/>
+    <tableColumn id="58" name="Res Force C_ROLLER_4-C_CAM"/>
+    <tableColumn id="59" name="Res Force C_ROLLER_5-C_CAM"/>
+    <tableColumn id="60" name="Res Force C_ROLLER_6-C_CAM"/>
+    <tableColumn id="61" name="Res Force L_ROLLER_10-PINION"/>
+    <tableColumn id="62" name="Res Force L_ROLLER_9-PINION"/>
+    <tableColumn id="63" name="Res Force L_ROLLER_8-PINION"/>
+    <tableColumn id="64" name="Res Force L_ROLLER_7-PINION"/>
+    <tableColumn id="65" name="Res Force L_ROLLER_6-PINION"/>
+    <tableColumn id="66" name="Res Force L_ROLLER_5-PINION"/>
+    <tableColumn id="67" name="Res Force L_ROLLER_4-PINION"/>
+    <tableColumn id="68" name="Res Force L_ROLLER_3-PINION"/>
+    <tableColumn id="69" name="Res Force L_ROLLER_2-PINION"/>
+    <tableColumn id="70" name="Res Force L_ROLLER_1-PINION"/>
+    <tableColumn id="71" name="Res Force L_ROLLER_6-L_RING"/>
+    <tableColumn id="72" name="Res Force L_ROLLER_5-L_RING"/>
+    <tableColumn id="73" name="Res Force L_ROLLER_4-L_RING"/>
+    <tableColumn id="74" name="Res Force L_ROLLER_3-L_RING"/>
+    <tableColumn id="75" name="Res Force L_ROLLER_2-L_RING"/>
+    <tableColumn id="76" name="Res Force L_ROLLER_1-L_RING"/>
+    <tableColumn id="77" name="Res Force Pinion-Collar-1"/>
+    <tableColumn id="78" name="Res Force Pinion-Collar-2"/>
+    <tableColumn id="79" name="Rear bracket force DS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="History" displayName="History" ref="A1:B2" totalsRowShown="0">
-  <autoFilter ref="A1:B2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="History__" displayName="History__" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
     <tableColumn id="1" name="time"/>
     <tableColumn id="2" name="runID"/>
@@ -560,13 +829,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:CA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:79">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,259 +923,813 @@
       <c r="AC1" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:79">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2">
+        <v>116</v>
+      </c>
+      <c r="AC2">
+        <v>63.7</v>
+      </c>
+      <c r="AD2">
+        <v>0.101</v>
+      </c>
+      <c r="AE2">
+        <v>0.076</v>
+      </c>
+      <c r="AF2">
+        <v>0.068</v>
+      </c>
+      <c r="AG2">
+        <v>0.124</v>
+      </c>
+      <c r="AH2">
+        <v>0.056</v>
+      </c>
+      <c r="AI2">
+        <v>0.081</v>
+      </c>
+      <c r="AT2">
+        <v>6.78</v>
+      </c>
+      <c r="AU2">
+        <v>0.468</v>
+      </c>
+      <c r="AV2">
+        <v>6.64</v>
+      </c>
+      <c r="AW2">
+        <v>0.061</v>
+      </c>
+      <c r="AX2">
+        <v>4.12</v>
+      </c>
+      <c r="AY2">
+        <v>0.654</v>
+      </c>
+      <c r="BA2">
+        <v>3.61</v>
+      </c>
+      <c r="BB2">
+        <v>63.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:79">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC3">
+        <v>81.8</v>
+      </c>
+      <c r="AD3">
+        <v>0.227</v>
+      </c>
+      <c r="AE3">
+        <v>0.186</v>
+      </c>
+      <c r="AF3">
+        <v>0.621</v>
+      </c>
+      <c r="AG3">
+        <v>0.424</v>
+      </c>
+      <c r="AH3">
+        <v>0.194</v>
+      </c>
+      <c r="AI3">
+        <v>0.247</v>
+      </c>
+      <c r="AJ3">
+        <v>5.59</v>
+      </c>
+      <c r="AK3">
+        <v>0.576</v>
+      </c>
+      <c r="AL3">
+        <v>7.13</v>
+      </c>
+      <c r="AM3">
+        <v>0.531</v>
+      </c>
+      <c r="AN3">
+        <v>8.039999999999999</v>
+      </c>
+      <c r="AO3">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="AP3">
+        <v>7.76</v>
+      </c>
+      <c r="AQ3">
+        <v>0.569</v>
+      </c>
+      <c r="AR3">
+        <v>5.19</v>
+      </c>
+      <c r="AS3">
+        <v>5.59</v>
+      </c>
+      <c r="AT3">
+        <v>8.039999999999999</v>
+      </c>
+      <c r="AU3">
+        <v>0.58</v>
+      </c>
+      <c r="AV3">
+        <v>7.76</v>
+      </c>
+      <c r="AW3">
+        <v>0.573</v>
+      </c>
+      <c r="AY3">
+        <v>0.136</v>
+      </c>
+      <c r="AZ3">
+        <v>1.3</v>
+      </c>
+      <c r="BA3">
+        <v>5.19</v>
+      </c>
+      <c r="BB3">
+        <v>81.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:79">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" t="s">
+        <v>115</v>
+      </c>
+      <c r="M4" t="s">
+        <v>117</v>
+      </c>
+      <c r="N4">
+        <v>22.6</v>
+      </c>
+      <c r="O4">
+        <v>24.9</v>
+      </c>
+      <c r="P4">
+        <v>1056.8</v>
+      </c>
+      <c r="Q4">
+        <v>1063.9</v>
+      </c>
+      <c r="R4">
+        <v>56.1</v>
+      </c>
+      <c r="S4">
+        <v>65.2</v>
+      </c>
+      <c r="T4">
+        <v>18.8</v>
+      </c>
+      <c r="U4">
+        <v>279.7</v>
+      </c>
+      <c r="V4">
+        <v>160.4</v>
+      </c>
+      <c r="W4">
+        <v>252.3</v>
+      </c>
+      <c r="X4">
+        <v>17.3</v>
+      </c>
+      <c r="Y4">
+        <v>1.92</v>
+      </c>
+      <c r="Z4">
+        <v>0.649</v>
+      </c>
+      <c r="AA4">
+        <v>11.9</v>
+      </c>
+      <c r="AB4">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:79">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC5">
+        <v>78.90000000000001</v>
+      </c>
+      <c r="AD5">
+        <v>0.161</v>
+      </c>
+      <c r="AE5">
+        <v>0.291</v>
+      </c>
+      <c r="AF5">
+        <v>0.514</v>
+      </c>
+      <c r="AG5">
+        <v>0.47</v>
+      </c>
+      <c r="AH5">
+        <v>0.066</v>
+      </c>
+      <c r="AI5">
+        <v>0.305</v>
+      </c>
+      <c r="AJ5">
+        <v>5.32</v>
+      </c>
+      <c r="AK5">
+        <v>0.656</v>
+      </c>
+      <c r="AL5">
+        <v>6.85</v>
+      </c>
+      <c r="AM5">
+        <v>0.572</v>
+      </c>
+      <c r="AN5">
+        <v>7.85</v>
+      </c>
+      <c r="AO5">
+        <v>0.591</v>
+      </c>
+      <c r="AP5">
+        <v>7.43</v>
+      </c>
+      <c r="AQ5">
+        <v>0.589</v>
+      </c>
+      <c r="AR5">
+        <v>4.76</v>
+      </c>
+      <c r="AS5">
+        <v>5.32</v>
+      </c>
+      <c r="AT5">
+        <v>7.85</v>
+      </c>
+      <c r="AU5">
+        <v>0.608</v>
+      </c>
+      <c r="AV5">
+        <v>7.43</v>
+      </c>
+      <c r="AW5">
+        <v>0.589</v>
+      </c>
+      <c r="AY5">
+        <v>0.173</v>
+      </c>
+      <c r="AZ5">
+        <v>0.173</v>
+      </c>
+      <c r="BA5">
+        <v>4.65</v>
+      </c>
+      <c r="BB5">
+        <v>78.90000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:79">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" t="s">
+        <v>118</v>
+      </c>
+      <c r="N6">
         <v>17.5</v>
       </c>
-      <c r="O2">
+      <c r="O6">
         <v>22.7</v>
       </c>
-      <c r="P2">
+      <c r="P6">
         <v>1226.8</v>
       </c>
-      <c r="Q2">
+      <c r="Q6">
         <v>1148.5</v>
       </c>
-      <c r="R2">
+      <c r="R6">
         <v>52.1</v>
       </c>
-      <c r="S2">
+      <c r="S6">
         <v>49.3</v>
       </c>
-      <c r="U2">
+      <c r="T6">
         <v>15</v>
       </c>
-      <c r="V2">
+      <c r="U6">
         <v>347.7</v>
       </c>
-      <c r="W2">
+      <c r="V6">
         <v>134.7</v>
       </c>
-      <c r="X2">
+      <c r="W6">
         <v>204.4</v>
       </c>
-      <c r="Y2">
+      <c r="X6">
         <v>14.4</v>
       </c>
-      <c r="Z2">
+      <c r="Y6">
         <v>1.11</v>
       </c>
-      <c r="AA2">
+      <c r="Z6">
         <v>0.586</v>
       </c>
-      <c r="AB2">
+      <c r="AA6">
         <v>10.7</v>
       </c>
-      <c r="AC2">
+      <c r="AB6">
         <v>12.7</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" t="s">
-        <v>49</v>
-      </c>
-      <c r="N3">
+    <row r="7" spans="1:79">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7" t="s">
+        <v>111</v>
+      </c>
+      <c r="L7" t="s">
+        <v>115</v>
+      </c>
+      <c r="M7" t="s">
+        <v>119</v>
+      </c>
+      <c r="N7">
         <v>16.3</v>
       </c>
-      <c r="O3">
+      <c r="O7">
         <v>17.3</v>
       </c>
-      <c r="P3">
+      <c r="P7">
         <v>1155.5</v>
       </c>
-      <c r="Q3">
+      <c r="Q7">
         <v>1029.7</v>
       </c>
-      <c r="R3">
+      <c r="R7">
         <v>42.6</v>
       </c>
-      <c r="S3">
+      <c r="S7">
         <v>39.3</v>
       </c>
-      <c r="T3">
+      <c r="T7">
+        <v>11.5</v>
+      </c>
+      <c r="U7">
+        <v>305.8</v>
+      </c>
+      <c r="V7">
+        <v>137.3</v>
+      </c>
+      <c r="W7">
+        <v>209.2</v>
+      </c>
+      <c r="X7">
+        <v>26.2</v>
+      </c>
+      <c r="Y7">
+        <v>0.732</v>
+      </c>
+      <c r="Z7">
+        <v>0.387</v>
+      </c>
+      <c r="AA7">
+        <v>9.25</v>
+      </c>
+      <c r="AB7">
+        <v>10.6</v>
+      </c>
+      <c r="CA7">
         <v>1.88</v>
       </c>
-      <c r="U3">
-        <v>11.5</v>
-      </c>
-      <c r="V3">
-        <v>305.8</v>
-      </c>
-      <c r="W3">
-        <v>137.3</v>
-      </c>
-      <c r="X3">
-        <v>209.2</v>
-      </c>
-      <c r="Y3">
-        <v>26.2</v>
-      </c>
-      <c r="Z3">
-        <v>0.732</v>
-      </c>
-      <c r="AA3">
-        <v>0.387</v>
-      </c>
-      <c r="AB3">
-        <v>9.25</v>
-      </c>
-      <c r="AC3">
-        <v>10.6</v>
-      </c>
     </row>
-    <row r="4" spans="1:29">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4">
+    <row r="8" spans="1:79">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" t="s">
+        <v>120</v>
+      </c>
+      <c r="N8">
         <v>18</v>
       </c>
-      <c r="O4">
+      <c r="O8">
         <v>22.8</v>
       </c>
-      <c r="P4">
+      <c r="P8">
         <v>1006.4</v>
       </c>
-      <c r="Q4">
+      <c r="Q8">
         <v>1011.8</v>
       </c>
-      <c r="R4">
+      <c r="R8">
         <v>65.3</v>
       </c>
-      <c r="S4">
+      <c r="S8">
         <v>63.1</v>
       </c>
-      <c r="U4">
+      <c r="T8">
         <v>14.3</v>
       </c>
-      <c r="V4">
+      <c r="U8">
         <v>332</v>
       </c>
-      <c r="W4">
+      <c r="V8">
         <v>173.6</v>
       </c>
-      <c r="X4">
+      <c r="W8">
         <v>224.4</v>
       </c>
-      <c r="Y4">
+      <c r="X8">
         <v>14.7</v>
       </c>
-      <c r="AB4">
+      <c r="AA8">
         <v>8.720000000000001</v>
       </c>
-      <c r="AC4">
+      <c r="AB8">
         <v>10.6</v>
       </c>
     </row>
@@ -920,7 +1743,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -932,18 +1755,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add panda profiling component
</commit_message>
<xml_diff>
--- a/database/MIT_database.xlsx
+++ b/database/MIT_database.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="213">
   <si>
     <t>RunID</t>
   </si>
@@ -104,6 +104,15 @@
     <t>Track sliding TS</t>
   </si>
   <si>
+    <t>Front bracket force DS</t>
+  </si>
+  <si>
+    <t>Front bracket force TS</t>
+  </si>
+  <si>
+    <t>Belt bracket force</t>
+  </si>
+  <si>
     <t>Backrest dynamic angle DS</t>
   </si>
   <si>
@@ -278,6 +287,45 @@
     <t>GR206405</t>
   </si>
   <si>
+    <t>GR208060</t>
+  </si>
+  <si>
+    <t>GR208381</t>
+  </si>
+  <si>
+    <t>GR208384</t>
+  </si>
+  <si>
+    <t>GR208388</t>
+  </si>
+  <si>
+    <t>GR208396</t>
+  </si>
+  <si>
+    <t>GR208527</t>
+  </si>
+  <si>
+    <t>GR208528</t>
+  </si>
+  <si>
+    <t>GR208530</t>
+  </si>
+  <si>
+    <t>GR208564</t>
+  </si>
+  <si>
+    <t>GR208591</t>
+  </si>
+  <si>
+    <t>GR208595</t>
+  </si>
+  <si>
+    <t>GR208960</t>
+  </si>
+  <si>
+    <t>GR208961</t>
+  </si>
+  <si>
     <t>GR208962</t>
   </si>
   <si>
@@ -332,12 +380,12 @@
     <t>unknown</t>
   </si>
   <si>
+    <t>10WP</t>
+  </si>
+  <si>
     <t>4WM</t>
   </si>
   <si>
-    <t>10WP</t>
-  </si>
-  <si>
     <t>Front Crash</t>
   </si>
   <si>
@@ -350,6 +398,9 @@
     <t>Luggage crash</t>
   </si>
   <si>
+    <t>ECE14</t>
+  </si>
+  <si>
     <t xml:space="preserve"> D95</t>
   </si>
   <si>
@@ -359,6 +410,12 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t xml:space="preserve"> D05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E14</t>
+  </si>
+  <si>
     <t>K04-0</t>
   </si>
   <si>
@@ -386,6 +443,9 @@
     <t>Unknown</t>
   </si>
   <si>
+    <t>Tracks:front most</t>
+  </si>
+  <si>
     <t>Tracks:rear most - 1 notch</t>
   </si>
   <si>
@@ -395,18 +455,27 @@
     <t xml:space="preserve"> HA:middle</t>
   </si>
   <si>
+    <t xml:space="preserve"> HA:upper most</t>
+  </si>
+  <si>
     <t xml:space="preserve"> HA:no_adjm</t>
   </si>
   <si>
     <t xml:space="preserve"> EuroNCAP40mph</t>
   </si>
   <si>
+    <t xml:space="preserve"> SPA2PULSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SPA2-RD8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EC17</t>
+  </si>
+  <si>
     <t xml:space="preserve"> FW56-Sinus</t>
   </si>
   <si>
-    <t xml:space="preserve"> SPA2-RD8</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Luggage-010</t>
   </si>
   <si>
@@ -437,18 +506,36 @@
     <t>__ _</t>
   </si>
   <si>
+    <t>FC95 MpDm</t>
+  </si>
+  <si>
+    <t>FC05 FmMp</t>
+  </si>
+  <si>
+    <t>RC95 RmDm</t>
+  </si>
+  <si>
+    <t>RC50 MpDm</t>
+  </si>
+  <si>
+    <t>LUG_ Rm-1nDm</t>
+  </si>
+  <si>
+    <t>FC05 MpUm</t>
+  </si>
+  <si>
+    <t>FC05 FmUm</t>
+  </si>
+  <si>
+    <t>FC50 RmUm</t>
+  </si>
+  <si>
+    <t>ECE14  RmDm</t>
+  </si>
+  <si>
     <t>FC50 Mp</t>
   </si>
   <si>
-    <t>RC50 MpDm</t>
-  </si>
-  <si>
-    <t>LUG_ Rm-1nDm</t>
-  </si>
-  <si>
-    <t>FC95 MpDm</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
@@ -521,6 +608,42 @@
     <t>08-01-2021 18:56:13</t>
   </si>
   <si>
+    <t>11-01-2021 09:17:44</t>
+  </si>
+  <si>
+    <t>11-01-2021 09:18:04</t>
+  </si>
+  <si>
+    <t>11-01-2021 09:26:32</t>
+  </si>
+  <si>
+    <t>11-01-2021 09:38:21</t>
+  </si>
+  <si>
+    <t>11-01-2021 09:50:36</t>
+  </si>
+  <si>
+    <t>11-01-2021 09:52:35</t>
+  </si>
+  <si>
+    <t>11-01-2021 09:53:40</t>
+  </si>
+  <si>
+    <t>11-01-2021 09:56:43</t>
+  </si>
+  <si>
+    <t>11-01-2021 09:59:59</t>
+  </si>
+  <si>
+    <t>11-01-2021 10:00:54</t>
+  </si>
+  <si>
+    <t>11-01-2021 10:02:14</t>
+  </si>
+  <si>
+    <t>11-01-2021 10:02:47</t>
+  </si>
+  <si>
     <t>GR206929,GR207006,GR207090</t>
   </si>
   <si>
@@ -528,6 +651,9 @@
   </si>
   <si>
     <t>GR206405,GR208962,GR208964</t>
+  </si>
+  <si>
+    <t>GR206405,GR206929,GR207006,GR207090,GR208060,GR208381,GR208384,GR208388,GR208396,GR208527,GR208528,GR208530,GR208564,GR208591,GR208595,GR208960,GR208961,GR208962,GR208964</t>
   </si>
 </sst>
 </file>
@@ -575,9 +701,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FEA" displayName="FEA" ref="A1:CE11" totalsRowShown="0">
-  <autoFilter ref="A1:CE11"/>
-  <tableColumns count="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FEA" displayName="FEA" ref="A1:CH24" totalsRowShown="0">
+  <autoFilter ref="A1:CH24"/>
+  <tableColumns count="86">
     <tableColumn id="1" name="RunID"/>
     <tableColumn id="2" name="OEM"/>
     <tableColumn id="3" name="project_name"/>
@@ -607,68 +733,71 @@
     <tableColumn id="27" name="Tilt Shear Force"/>
     <tableColumn id="28" name="Track sliding DS"/>
     <tableColumn id="29" name="Track sliding TS"/>
-    <tableColumn id="30" name="Backrest dynamic angle DS"/>
-    <tableColumn id="31" name="Backrest dynamic angle TS"/>
-    <tableColumn id="32" name="Backrest static angle DS"/>
-    <tableColumn id="33" name="Backrest static angle TS"/>
-    <tableColumn id="34" name="Pinion torque"/>
-    <tableColumn id="35" name="Res_F C_ROLLER_1-C_CAM"/>
-    <tableColumn id="36" name="Res_F C_ROLLER_2-C_CAM"/>
-    <tableColumn id="37" name="Res_F C_ROLLER_3-C_CAM"/>
-    <tableColumn id="38" name="Res_F C_ROLLER_4-C_CAM"/>
-    <tableColumn id="39" name="Res_F C_ROLLER_5-C_CAM"/>
-    <tableColumn id="40" name="Res_F C_ROLLER_6-C_CAM"/>
-    <tableColumn id="41" name="Res_F L_ROLLER_10-PINION"/>
-    <tableColumn id="42" name="Res_F L_ROLLER_9-PINION"/>
-    <tableColumn id="43" name="Res_F L_ROLLER_8-PINION"/>
-    <tableColumn id="44" name="Res_F L_ROLLER_7-PINION"/>
-    <tableColumn id="45" name="Res_F L_ROLLER_6-PINION"/>
-    <tableColumn id="46" name="Res_F L_ROLLER_5-PINION"/>
-    <tableColumn id="47" name="Res_F L_ROLLER_4-PINION"/>
-    <tableColumn id="48" name="Res_F L_ROLLER_3-PINION"/>
-    <tableColumn id="49" name="Res_F L_ROLLER_2-PINION"/>
-    <tableColumn id="50" name="Res_F L_ROLLER_1-PINION"/>
-    <tableColumn id="51" name="Res_F L_ROLLER_6-L_RING"/>
-    <tableColumn id="52" name="Res_F L_ROLLER_5-L_RING"/>
-    <tableColumn id="53" name="Res_F L_ROLLER_4-L_RING"/>
-    <tableColumn id="54" name="Res_F L_ROLLER_3-L_RING"/>
-    <tableColumn id="55" name="Res_F L_ROLLER_2-L_RING"/>
-    <tableColumn id="56" name="Res_F L_ROLLER_1-L_RING"/>
-    <tableColumn id="57" name="Res_F Pinion-Collar-1"/>
-    <tableColumn id="58" name="Res_F Pinion-Collar-2"/>
-    <tableColumn id="59" name="Torque MX on pinions section"/>
-    <tableColumn id="60" name="Res Force C_ROLLER_1-C_CAM"/>
-    <tableColumn id="61" name="Res Force C_ROLLER_2-C_CAM"/>
-    <tableColumn id="62" name="Res Force C_ROLLER_3-C_CAM"/>
-    <tableColumn id="63" name="Res Force C_ROLLER_4-C_CAM"/>
-    <tableColumn id="64" name="Res Force C_ROLLER_5-C_CAM"/>
-    <tableColumn id="65" name="Res Force C_ROLLER_6-C_CAM"/>
-    <tableColumn id="66" name="Res Force L_ROLLER_10-PINION"/>
-    <tableColumn id="67" name="Res Force L_ROLLER_9-PINION"/>
-    <tableColumn id="68" name="Res Force L_ROLLER_8-PINION"/>
-    <tableColumn id="69" name="Res Force L_ROLLER_7-PINION"/>
-    <tableColumn id="70" name="Res Force L_ROLLER_6-PINION"/>
-    <tableColumn id="71" name="Res Force L_ROLLER_5-PINION"/>
-    <tableColumn id="72" name="Res Force L_ROLLER_4-PINION"/>
-    <tableColumn id="73" name="Res Force L_ROLLER_3-PINION"/>
-    <tableColumn id="74" name="Res Force L_ROLLER_2-PINION"/>
-    <tableColumn id="75" name="Res Force L_ROLLER_1-PINION"/>
-    <tableColumn id="76" name="Res Force L_ROLLER_6-L_RING"/>
-    <tableColumn id="77" name="Res Force L_ROLLER_5-L_RING"/>
-    <tableColumn id="78" name="Res Force L_ROLLER_4-L_RING"/>
-    <tableColumn id="79" name="Res Force L_ROLLER_3-L_RING"/>
-    <tableColumn id="80" name="Res Force L_ROLLER_2-L_RING"/>
-    <tableColumn id="81" name="Res Force L_ROLLER_1-L_RING"/>
-    <tableColumn id="82" name="Res Force Pinion-Collar-1"/>
-    <tableColumn id="83" name="Res Force Pinion-Collar-2"/>
+    <tableColumn id="30" name="Front bracket force DS"/>
+    <tableColumn id="31" name="Front bracket force TS"/>
+    <tableColumn id="32" name="Belt bracket force"/>
+    <tableColumn id="33" name="Backrest dynamic angle DS"/>
+    <tableColumn id="34" name="Backrest dynamic angle TS"/>
+    <tableColumn id="35" name="Backrest static angle DS"/>
+    <tableColumn id="36" name="Backrest static angle TS"/>
+    <tableColumn id="37" name="Pinion torque"/>
+    <tableColumn id="38" name="Res_F C_ROLLER_1-C_CAM"/>
+    <tableColumn id="39" name="Res_F C_ROLLER_2-C_CAM"/>
+    <tableColumn id="40" name="Res_F C_ROLLER_3-C_CAM"/>
+    <tableColumn id="41" name="Res_F C_ROLLER_4-C_CAM"/>
+    <tableColumn id="42" name="Res_F C_ROLLER_5-C_CAM"/>
+    <tableColumn id="43" name="Res_F C_ROLLER_6-C_CAM"/>
+    <tableColumn id="44" name="Res_F L_ROLLER_10-PINION"/>
+    <tableColumn id="45" name="Res_F L_ROLLER_9-PINION"/>
+    <tableColumn id="46" name="Res_F L_ROLLER_8-PINION"/>
+    <tableColumn id="47" name="Res_F L_ROLLER_7-PINION"/>
+    <tableColumn id="48" name="Res_F L_ROLLER_6-PINION"/>
+    <tableColumn id="49" name="Res_F L_ROLLER_5-PINION"/>
+    <tableColumn id="50" name="Res_F L_ROLLER_4-PINION"/>
+    <tableColumn id="51" name="Res_F L_ROLLER_3-PINION"/>
+    <tableColumn id="52" name="Res_F L_ROLLER_2-PINION"/>
+    <tableColumn id="53" name="Res_F L_ROLLER_1-PINION"/>
+    <tableColumn id="54" name="Res_F L_ROLLER_6-L_RING"/>
+    <tableColumn id="55" name="Res_F L_ROLLER_5-L_RING"/>
+    <tableColumn id="56" name="Res_F L_ROLLER_4-L_RING"/>
+    <tableColumn id="57" name="Res_F L_ROLLER_3-L_RING"/>
+    <tableColumn id="58" name="Res_F L_ROLLER_2-L_RING"/>
+    <tableColumn id="59" name="Res_F L_ROLLER_1-L_RING"/>
+    <tableColumn id="60" name="Res_F Pinion-Collar-1"/>
+    <tableColumn id="61" name="Res_F Pinion-Collar-2"/>
+    <tableColumn id="62" name="Torque MX on pinions section"/>
+    <tableColumn id="63" name="Res Force C_ROLLER_1-C_CAM"/>
+    <tableColumn id="64" name="Res Force C_ROLLER_2-C_CAM"/>
+    <tableColumn id="65" name="Res Force C_ROLLER_3-C_CAM"/>
+    <tableColumn id="66" name="Res Force C_ROLLER_4-C_CAM"/>
+    <tableColumn id="67" name="Res Force C_ROLLER_5-C_CAM"/>
+    <tableColumn id="68" name="Res Force C_ROLLER_6-C_CAM"/>
+    <tableColumn id="69" name="Res Force L_ROLLER_10-PINION"/>
+    <tableColumn id="70" name="Res Force L_ROLLER_9-PINION"/>
+    <tableColumn id="71" name="Res Force L_ROLLER_8-PINION"/>
+    <tableColumn id="72" name="Res Force L_ROLLER_7-PINION"/>
+    <tableColumn id="73" name="Res Force L_ROLLER_6-PINION"/>
+    <tableColumn id="74" name="Res Force L_ROLLER_5-PINION"/>
+    <tableColumn id="75" name="Res Force L_ROLLER_4-PINION"/>
+    <tableColumn id="76" name="Res Force L_ROLLER_3-PINION"/>
+    <tableColumn id="77" name="Res Force L_ROLLER_2-PINION"/>
+    <tableColumn id="78" name="Res Force L_ROLLER_1-PINION"/>
+    <tableColumn id="79" name="Res Force L_ROLLER_6-L_RING"/>
+    <tableColumn id="80" name="Res Force L_ROLLER_5-L_RING"/>
+    <tableColumn id="81" name="Res Force L_ROLLER_4-L_RING"/>
+    <tableColumn id="82" name="Res Force L_ROLLER_3-L_RING"/>
+    <tableColumn id="83" name="Res Force L_ROLLER_2-L_RING"/>
+    <tableColumn id="84" name="Res Force L_ROLLER_1-L_RING"/>
+    <tableColumn id="85" name="Res Force Pinion-Collar-1"/>
+    <tableColumn id="86" name="Res Force Pinion-Collar-2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="History__" displayName="History__" ref="A1:B23" totalsRowShown="0">
-  <autoFilter ref="A1:B23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="History__" displayName="History__" ref="A1:B35" totalsRowShown="0">
+  <autoFilter ref="A1:B35"/>
   <tableColumns count="2">
     <tableColumn id="1" name="time"/>
     <tableColumn id="2" name="runID"/>
@@ -962,13 +1091,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CE11"/>
+  <dimension ref="A1:CH24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:83">
+    <row r="1" spans="1:86">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1218,46 +1347,55 @@
       <c r="CE1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:83">
+      <c r="CF1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:86">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="H2" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="I2" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="J2" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="L2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="M2" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="N2">
         <v>17.5</v>
@@ -1305,45 +1443,45 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="3" spans="1:83">
+    <row r="3" spans="1:86">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="F3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="G3" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="H3" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="I3" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="J3" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="K3" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="L3" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="M3" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="N3">
         <v>16.3</v>
@@ -1394,45 +1532,45 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="4" spans="1:83">
+    <row r="4" spans="1:86">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="G4" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="H4" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="I4" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="J4" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="K4" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="L4" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="M4" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="N4">
         <v>18</v>
@@ -1474,575 +1612,1675 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="5" spans="1:83">
+    <row r="5" spans="1:86">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K5" t="s">
+        <v>156</v>
+      </c>
+      <c r="L5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:86">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J6" t="s">
+        <v>148</v>
+      </c>
+      <c r="K6" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" t="s">
+        <v>154</v>
+      </c>
+      <c r="M6" t="s">
+        <v>161</v>
+      </c>
+      <c r="N6">
+        <v>15.6</v>
+      </c>
+      <c r="O6">
+        <v>20.1</v>
+      </c>
+      <c r="P6">
+        <v>1081.9</v>
+      </c>
+      <c r="Q6">
+        <v>998.8</v>
+      </c>
+      <c r="R6">
+        <v>65.5</v>
+      </c>
+      <c r="S6">
+        <v>67.7</v>
+      </c>
+      <c r="U6">
+        <v>14.2</v>
+      </c>
+      <c r="V6">
+        <v>348.1</v>
+      </c>
+      <c r="W6">
+        <v>179.1</v>
+      </c>
+      <c r="X6">
+        <v>214.3</v>
+      </c>
+      <c r="Y6">
+        <v>18.3</v>
+      </c>
+      <c r="Z6">
+        <v>2.3</v>
+      </c>
+      <c r="AA6">
+        <v>0.297</v>
+      </c>
+      <c r="AB6">
+        <v>8.92</v>
+      </c>
+      <c r="AC6">
+        <v>12.6</v>
+      </c>
+      <c r="AD6">
+        <v>10</v>
+      </c>
+      <c r="AE6">
+        <v>7.5</v>
+      </c>
+      <c r="AF6">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:86">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I7" t="s">
+        <v>144</v>
+      </c>
+      <c r="J7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K7" t="s">
+        <v>155</v>
+      </c>
+      <c r="L7" t="s">
+        <v>154</v>
+      </c>
+      <c r="M7" t="s">
+        <v>163</v>
+      </c>
+      <c r="N7">
+        <v>18</v>
+      </c>
+      <c r="O7">
+        <v>22.3</v>
+      </c>
+      <c r="P7">
+        <v>1073.6</v>
+      </c>
+      <c r="Q7">
+        <v>1034.4</v>
+      </c>
+      <c r="R7">
+        <v>47.4</v>
+      </c>
+      <c r="S7">
+        <v>54.6</v>
+      </c>
+      <c r="U7">
+        <v>16.1</v>
+      </c>
+      <c r="V7">
+        <v>327.6</v>
+      </c>
+      <c r="W7">
+        <v>125.4</v>
+      </c>
+      <c r="X7">
+        <v>220.6</v>
+      </c>
+      <c r="Y7">
+        <v>24.2</v>
+      </c>
+      <c r="Z7">
+        <v>2.11</v>
+      </c>
+      <c r="AA7">
+        <v>0.312</v>
+      </c>
+      <c r="AB7">
+        <v>10.6</v>
+      </c>
+      <c r="AC7">
+        <v>13.5</v>
+      </c>
+      <c r="AD7">
+        <v>15.4</v>
+      </c>
+      <c r="AE7">
+        <v>9.720000000000001</v>
+      </c>
+      <c r="AF7">
+        <v>16.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:86">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" t="s">
+        <v>145</v>
+      </c>
+      <c r="J8" t="s">
+        <v>148</v>
+      </c>
+      <c r="K8" t="s">
+        <v>155</v>
+      </c>
+      <c r="L8" t="s">
+        <v>157</v>
+      </c>
+      <c r="M8" t="s">
+        <v>160</v>
+      </c>
+      <c r="N8">
+        <v>16.6</v>
+      </c>
+      <c r="O8">
+        <v>18.6</v>
+      </c>
+      <c r="P8">
+        <v>1227.9</v>
+      </c>
+      <c r="Q8">
+        <v>1068.1</v>
+      </c>
+      <c r="R8">
+        <v>42.9</v>
+      </c>
+      <c r="S8">
+        <v>39.9</v>
+      </c>
+      <c r="T8">
+        <v>1.97</v>
+      </c>
+      <c r="U8">
+        <v>11.7</v>
+      </c>
+      <c r="V8">
+        <v>312.1</v>
+      </c>
+      <c r="W8">
+        <v>138.1</v>
+      </c>
+      <c r="X8">
+        <v>198</v>
+      </c>
+      <c r="Y8">
+        <v>24.9</v>
+      </c>
+      <c r="Z8">
+        <v>0.534</v>
+      </c>
+      <c r="AA8">
+        <v>0.449</v>
+      </c>
+      <c r="AB8">
+        <v>9.52</v>
+      </c>
+      <c r="AC8">
+        <v>11.2</v>
+      </c>
+      <c r="AD8">
+        <v>10.1</v>
+      </c>
+      <c r="AE8">
+        <v>6.59</v>
+      </c>
+      <c r="AF8">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:86">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" t="s">
+        <v>145</v>
+      </c>
+      <c r="J9" t="s">
+        <v>148</v>
+      </c>
+      <c r="K9" t="s">
+        <v>155</v>
+      </c>
+      <c r="L9" t="s">
+        <v>157</v>
+      </c>
+      <c r="M9" t="s">
+        <v>164</v>
+      </c>
+      <c r="N9">
+        <v>1.46</v>
+      </c>
+      <c r="O9">
+        <v>4.55</v>
+      </c>
+      <c r="P9">
+        <v>1295.7</v>
+      </c>
+      <c r="Q9">
+        <v>1153</v>
+      </c>
+      <c r="R9">
+        <v>25.4</v>
+      </c>
+      <c r="S9">
+        <v>36.9</v>
+      </c>
+      <c r="U9">
+        <v>6.3</v>
+      </c>
+      <c r="V9">
+        <v>225.4</v>
+      </c>
+      <c r="W9">
+        <v>153.8</v>
+      </c>
+      <c r="X9">
+        <v>165.8</v>
+      </c>
+      <c r="Y9">
+        <v>33</v>
+      </c>
+      <c r="Z9">
+        <v>0.172</v>
+      </c>
+      <c r="AA9">
+        <v>0.136</v>
+      </c>
+      <c r="AB9">
+        <v>4.77</v>
+      </c>
+      <c r="AC9">
+        <v>6.46</v>
+      </c>
+      <c r="AD9">
+        <v>8.19</v>
+      </c>
+      <c r="AE9">
+        <v>6.11</v>
+      </c>
+      <c r="AF9">
+        <v>7.31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:86">
+      <c r="A10" t="s">
         <v>94</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" t="s">
+        <v>139</v>
+      </c>
+      <c r="I10" t="s">
+        <v>144</v>
+      </c>
+      <c r="J10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K10" t="s">
+        <v>155</v>
+      </c>
+      <c r="L10" t="s">
+        <v>154</v>
+      </c>
+      <c r="M10" t="s">
+        <v>159</v>
+      </c>
+      <c r="N10">
+        <v>19.2</v>
+      </c>
+      <c r="O10">
+        <v>22.7</v>
+      </c>
+      <c r="P10">
+        <v>1194.6</v>
+      </c>
+      <c r="Q10">
+        <v>1168.1</v>
+      </c>
+      <c r="R10">
+        <v>50.7</v>
+      </c>
+      <c r="S10">
+        <v>47.3</v>
+      </c>
+      <c r="U10">
+        <v>15</v>
+      </c>
+      <c r="V10">
+        <v>326.7</v>
+      </c>
+      <c r="W10">
+        <v>132.9</v>
+      </c>
+      <c r="X10">
+        <v>199.5</v>
+      </c>
+      <c r="Y10">
+        <v>11.9</v>
+      </c>
+      <c r="Z10">
+        <v>1.4</v>
+      </c>
+      <c r="AA10">
+        <v>0.504</v>
+      </c>
+      <c r="AB10">
+        <v>11.8</v>
+      </c>
+      <c r="AC10">
+        <v>13</v>
+      </c>
+      <c r="AD10">
+        <v>15.6</v>
+      </c>
+      <c r="AE10">
+        <v>10.7</v>
+      </c>
+      <c r="AF10">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:86">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I11" t="s">
+        <v>144</v>
+      </c>
+      <c r="J11" t="s">
+        <v>149</v>
+      </c>
+      <c r="K11" t="s">
+        <v>157</v>
+      </c>
+      <c r="L11" t="s">
+        <v>156</v>
+      </c>
+      <c r="M11" t="s">
+        <v>165</v>
+      </c>
+      <c r="O11">
+        <v>7.12</v>
+      </c>
+      <c r="P11">
+        <v>1795.3</v>
+      </c>
+      <c r="Q11">
+        <v>1958.1</v>
+      </c>
+      <c r="V11">
+        <v>69.7</v>
+      </c>
+      <c r="X11">
+        <v>187.2</v>
+      </c>
+      <c r="Y11">
+        <v>23.1</v>
+      </c>
+      <c r="AD11">
+        <v>16</v>
+      </c>
+      <c r="AE11">
+        <v>13.9</v>
+      </c>
+      <c r="AF11">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="12" spans="1:86">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" t="s">
+        <v>140</v>
+      </c>
+      <c r="I12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K12" t="s">
+        <v>157</v>
+      </c>
+      <c r="L12" t="s">
+        <v>154</v>
+      </c>
+      <c r="M12" t="s">
+        <v>166</v>
+      </c>
+      <c r="N12">
+        <v>14.9</v>
+      </c>
+      <c r="O12">
+        <v>13.9</v>
+      </c>
+      <c r="P12">
+        <v>2142.9</v>
+      </c>
+      <c r="Q12">
+        <v>2125.9</v>
+      </c>
+      <c r="V12">
+        <v>42.3</v>
+      </c>
+      <c r="X12">
+        <v>229.5</v>
+      </c>
+      <c r="Y12">
+        <v>28.2</v>
+      </c>
+      <c r="Z12">
+        <v>1.69</v>
+      </c>
+      <c r="AA12">
+        <v>0.349</v>
+      </c>
+      <c r="AD12">
+        <v>14.3</v>
+      </c>
+      <c r="AE12">
+        <v>15.2</v>
+      </c>
+      <c r="AF12">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:86">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" t="s">
+        <v>143</v>
+      </c>
+      <c r="I13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J13" t="s">
+        <v>151</v>
+      </c>
+      <c r="K13" t="s">
+        <v>155</v>
+      </c>
+      <c r="L13" t="s">
+        <v>155</v>
+      </c>
+      <c r="M13" t="s">
+        <v>167</v>
+      </c>
+      <c r="N13">
+        <v>5.65</v>
+      </c>
+      <c r="O13">
+        <v>5.98</v>
+      </c>
+      <c r="P13">
+        <v>2006.6</v>
+      </c>
+      <c r="Q13">
+        <v>1796.9</v>
+      </c>
+      <c r="V13">
+        <v>156.2</v>
+      </c>
+      <c r="W13">
+        <v>255.5</v>
+      </c>
+      <c r="Z13">
+        <v>0.249</v>
+      </c>
+      <c r="AA13">
+        <v>0.111</v>
+      </c>
+      <c r="AD13">
+        <v>11.6</v>
+      </c>
+      <c r="AE13">
+        <v>10.8</v>
+      </c>
+      <c r="AF13">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:86">
+      <c r="A14" t="s">
         <v>98</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" t="s">
+        <v>140</v>
+      </c>
+      <c r="I14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J14" t="s">
+        <v>148</v>
+      </c>
+      <c r="K14" t="s">
+        <v>155</v>
+      </c>
+      <c r="L14" t="s">
+        <v>155</v>
+      </c>
+      <c r="M14" t="s">
+        <v>168</v>
+      </c>
+      <c r="N14">
+        <v>14</v>
+      </c>
+      <c r="O14">
+        <v>16</v>
+      </c>
+      <c r="P14">
+        <v>1219</v>
+      </c>
+      <c r="Q14">
+        <v>1092.7</v>
+      </c>
+      <c r="R14">
+        <v>26.8</v>
+      </c>
+      <c r="S14">
+        <v>38.4</v>
+      </c>
+      <c r="T14">
+        <v>2.2</v>
+      </c>
+      <c r="U14">
+        <v>8.24</v>
+      </c>
+      <c r="V14">
+        <v>121.8</v>
+      </c>
+      <c r="W14">
+        <v>133.4</v>
+      </c>
+      <c r="X14">
+        <v>168</v>
+      </c>
+      <c r="Y14">
+        <v>20.9</v>
+      </c>
+      <c r="Z14">
+        <v>1.44</v>
+      </c>
+      <c r="AA14">
+        <v>0.168</v>
+      </c>
+      <c r="AB14">
+        <v>7.09</v>
+      </c>
+      <c r="AC14">
+        <v>9.789999999999999</v>
+      </c>
+      <c r="AD14">
+        <v>11.4</v>
+      </c>
+      <c r="AE14">
+        <v>6.52</v>
+      </c>
+      <c r="AF14">
+        <v>8.359999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:86">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" t="s">
+        <v>142</v>
+      </c>
+      <c r="I15" t="s">
+        <v>146</v>
+      </c>
+      <c r="J15" t="s">
+        <v>148</v>
+      </c>
+      <c r="K15" t="s">
+        <v>155</v>
+      </c>
+      <c r="L15" t="s">
+        <v>155</v>
+      </c>
+      <c r="M15" t="s">
+        <v>169</v>
+      </c>
+      <c r="N15">
+        <v>3.28</v>
+      </c>
+      <c r="O15">
+        <v>4.24</v>
+      </c>
+      <c r="P15">
+        <v>1110.5</v>
+      </c>
+      <c r="Q15">
+        <v>1158.7</v>
+      </c>
+      <c r="R15">
+        <v>21.6</v>
+      </c>
+      <c r="S15">
+        <v>36.7</v>
+      </c>
+      <c r="U15">
+        <v>6.06</v>
+      </c>
+      <c r="V15">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="W15">
+        <v>144.3</v>
+      </c>
+      <c r="X15">
+        <v>176.8</v>
+      </c>
+      <c r="Y15">
+        <v>47</v>
+      </c>
+      <c r="Z15">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="AA15">
+        <v>0.149</v>
+      </c>
+      <c r="AB15">
+        <v>5.08</v>
+      </c>
+      <c r="AC15">
+        <v>6.25</v>
+      </c>
+      <c r="AD15">
+        <v>7.74</v>
+      </c>
+      <c r="AE15">
+        <v>5.25</v>
+      </c>
+      <c r="AF15">
+        <v>6.97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:86">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I16" t="s">
+        <v>146</v>
+      </c>
+      <c r="J16" t="s">
+        <v>148</v>
+      </c>
+      <c r="K16" t="s">
+        <v>157</v>
+      </c>
+      <c r="L16" t="s">
+        <v>157</v>
+      </c>
+      <c r="M16" t="s">
+        <v>170</v>
+      </c>
+      <c r="N16">
+        <v>14.8</v>
+      </c>
+      <c r="O16">
+        <v>15</v>
+      </c>
+      <c r="P16">
+        <v>1088.5</v>
+      </c>
+      <c r="Q16">
+        <v>1027.9</v>
+      </c>
+      <c r="R16">
+        <v>55.4</v>
+      </c>
+      <c r="S16">
+        <v>62.3</v>
+      </c>
+      <c r="T16">
+        <v>2.38</v>
+      </c>
+      <c r="U16">
+        <v>11.8</v>
+      </c>
+      <c r="V16">
+        <v>135.4</v>
+      </c>
+      <c r="W16">
+        <v>171.8</v>
+      </c>
+      <c r="X16">
+        <v>217.7</v>
+      </c>
+      <c r="Y16">
+        <v>30.8</v>
+      </c>
+      <c r="Z16">
+        <v>0.713</v>
+      </c>
+      <c r="AA16">
+        <v>0.412</v>
+      </c>
+      <c r="AB16">
+        <v>7.37</v>
+      </c>
+      <c r="AC16">
+        <v>9.43</v>
+      </c>
+      <c r="AD16">
+        <v>10.3</v>
+      </c>
+      <c r="AE16">
+        <v>4.87</v>
+      </c>
+      <c r="AF16">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:62">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" t="s">
+        <v>132</v>
+      </c>
+      <c r="G17" t="s">
+        <v>133</v>
+      </c>
+      <c r="H17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I17" t="s">
+        <v>144</v>
+      </c>
+      <c r="J17" t="s">
+        <v>130</v>
+      </c>
+      <c r="K17" t="s">
+        <v>156</v>
+      </c>
+      <c r="L17" t="s">
+        <v>155</v>
+      </c>
+      <c r="M17" t="s">
+        <v>171</v>
+      </c>
+      <c r="N17">
+        <v>10.5</v>
+      </c>
+      <c r="O17">
+        <v>12.9</v>
+      </c>
+      <c r="P17">
+        <v>423.9</v>
+      </c>
+      <c r="Q17">
+        <v>324.6</v>
+      </c>
+      <c r="V17">
+        <v>264.3</v>
+      </c>
+      <c r="Z17">
+        <v>2.2</v>
+      </c>
+      <c r="AA17">
+        <v>0.218</v>
+      </c>
+      <c r="AD17">
+        <v>9.24</v>
+      </c>
+      <c r="AE17">
+        <v>1.82</v>
+      </c>
+      <c r="AF17">
+        <v>8.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:62">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G18" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I18" t="s">
+        <v>141</v>
+      </c>
+      <c r="J18" t="s">
+        <v>130</v>
+      </c>
+      <c r="K18" t="s">
+        <v>156</v>
+      </c>
+      <c r="L18" t="s">
+        <v>156</v>
+      </c>
+      <c r="M18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:62">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" t="s">
+        <v>147</v>
+      </c>
+      <c r="J19" t="s">
+        <v>152</v>
+      </c>
+      <c r="K19" t="s">
+        <v>156</v>
+      </c>
+      <c r="L19" t="s">
+        <v>156</v>
+      </c>
+      <c r="M19" t="s">
+        <v>172</v>
+      </c>
+      <c r="X19">
+        <v>161.3</v>
+      </c>
+      <c r="Y19">
+        <v>74.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:62">
+      <c r="A20" t="s">
         <v>104</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" t="s">
+        <v>140</v>
+      </c>
+      <c r="I20" t="s">
+        <v>144</v>
+      </c>
+      <c r="J20" t="s">
+        <v>150</v>
+      </c>
+      <c r="K20" t="s">
+        <v>157</v>
+      </c>
+      <c r="L20" t="s">
+        <v>155</v>
+      </c>
+      <c r="M20" t="s">
+        <v>166</v>
+      </c>
+      <c r="N20">
+        <v>14.9</v>
+      </c>
+      <c r="O20">
+        <v>14.5</v>
+      </c>
+      <c r="P20">
+        <v>2182.8</v>
+      </c>
+      <c r="Q20">
+        <v>2279.4</v>
+      </c>
+      <c r="V20">
+        <v>50.3</v>
+      </c>
+      <c r="X20">
+        <v>231.3</v>
+      </c>
+      <c r="Y20">
+        <v>31.6</v>
+      </c>
+      <c r="Z20">
+        <v>3.69</v>
+      </c>
+      <c r="AA20">
+        <v>0.38</v>
+      </c>
+      <c r="AG20">
+        <v>22.6</v>
+      </c>
+      <c r="AH20">
+        <v>19.4</v>
+      </c>
+      <c r="AI20">
+        <v>12.6</v>
+      </c>
+      <c r="AJ20">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:62">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" t="s">
+        <v>143</v>
+      </c>
+      <c r="I21" t="s">
+        <v>144</v>
+      </c>
+      <c r="J21" t="s">
+        <v>153</v>
+      </c>
+      <c r="K21" t="s">
+        <v>155</v>
+      </c>
+      <c r="L21" t="s">
+        <v>158</v>
+      </c>
+      <c r="M21" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK21">
+        <v>63.7</v>
+      </c>
+      <c r="AL21">
+        <v>0.101</v>
+      </c>
+      <c r="AM21">
+        <v>0.076</v>
+      </c>
+      <c r="AN21">
+        <v>0.068</v>
+      </c>
+      <c r="AO21">
+        <v>0.124</v>
+      </c>
+      <c r="AP21">
+        <v>0.056</v>
+      </c>
+      <c r="AQ21">
+        <v>0.081</v>
+      </c>
+      <c r="BB21">
+        <v>6.78</v>
+      </c>
+      <c r="BC21">
+        <v>0.468</v>
+      </c>
+      <c r="BD21">
+        <v>6.64</v>
+      </c>
+      <c r="BE21">
+        <v>0.061</v>
+      </c>
+      <c r="BF21">
+        <v>4.12</v>
+      </c>
+      <c r="BG21">
+        <v>0.654</v>
+      </c>
+      <c r="BI21">
+        <v>3.61</v>
+      </c>
+      <c r="BJ21">
+        <v>63.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:62">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J22" t="s">
+        <v>153</v>
+      </c>
+      <c r="K22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L22" t="s">
+        <v>154</v>
+      </c>
+      <c r="M22" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK22">
+        <v>81.8</v>
+      </c>
+      <c r="AL22">
+        <v>0.227</v>
+      </c>
+      <c r="AM22">
+        <v>0.186</v>
+      </c>
+      <c r="AN22">
+        <v>0.621</v>
+      </c>
+      <c r="AO22">
+        <v>0.424</v>
+      </c>
+      <c r="AP22">
+        <v>0.194</v>
+      </c>
+      <c r="AQ22">
+        <v>0.247</v>
+      </c>
+      <c r="AR22">
+        <v>5.59</v>
+      </c>
+      <c r="AS22">
+        <v>0.576</v>
+      </c>
+      <c r="AT22">
+        <v>7.13</v>
+      </c>
+      <c r="AU22">
+        <v>0.531</v>
+      </c>
+      <c r="AV22">
+        <v>8.039999999999999</v>
+      </c>
+      <c r="AW22">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="AX22">
+        <v>7.76</v>
+      </c>
+      <c r="AY22">
+        <v>0.569</v>
+      </c>
+      <c r="AZ22">
+        <v>5.19</v>
+      </c>
+      <c r="BA22">
+        <v>5.59</v>
+      </c>
+      <c r="BB22">
+        <v>8.039999999999999</v>
+      </c>
+      <c r="BC22">
+        <v>0.58</v>
+      </c>
+      <c r="BD22">
+        <v>7.76</v>
+      </c>
+      <c r="BE22">
+        <v>0.573</v>
+      </c>
+      <c r="BG22">
+        <v>0.136</v>
+      </c>
+      <c r="BH22">
+        <v>1.3</v>
+      </c>
+      <c r="BI22">
+        <v>5.19</v>
+      </c>
+      <c r="BJ22">
+        <v>81.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:62">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" t="s">
+        <v>144</v>
+      </c>
+      <c r="J23" t="s">
+        <v>148</v>
+      </c>
+      <c r="K23" t="s">
+        <v>154</v>
+      </c>
+      <c r="L23" t="s">
+        <v>157</v>
+      </c>
+      <c r="M23" t="s">
+        <v>163</v>
+      </c>
+      <c r="N23">
+        <v>22.6</v>
+      </c>
+      <c r="O23">
+        <v>24.9</v>
+      </c>
+      <c r="P23">
+        <v>1056.8</v>
+      </c>
+      <c r="Q23">
+        <v>1063.9</v>
+      </c>
+      <c r="R23">
+        <v>56.1</v>
+      </c>
+      <c r="S23">
+        <v>65.2</v>
+      </c>
+      <c r="U23">
+        <v>18.8</v>
+      </c>
+      <c r="V23">
+        <v>279.7</v>
+      </c>
+      <c r="W23">
+        <v>160.4</v>
+      </c>
+      <c r="X23">
+        <v>252.3</v>
+      </c>
+      <c r="Y23">
+        <v>17.3</v>
+      </c>
+      <c r="Z23">
+        <v>1.92</v>
+      </c>
+      <c r="AA23">
+        <v>0.649</v>
+      </c>
+      <c r="AB23">
+        <v>11.9</v>
+      </c>
+      <c r="AC23">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:62">
+      <c r="A24" t="s">
         <v>108</v>
       </c>
-      <c r="F5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" t="s">
-        <v>115</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" t="s">
         <v>122</v>
       </c>
-      <c r="I5" t="s">
-        <v>122</v>
-      </c>
-      <c r="J5" t="s">
-        <v>113</v>
-      </c>
-      <c r="K5" t="s">
-        <v>133</v>
-      </c>
-      <c r="L5" t="s">
-        <v>133</v>
-      </c>
-      <c r="M5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:83">
-      <c r="A6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H6" t="s">
-        <v>121</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="E24" t="s">
         <v>126</v>
       </c>
-      <c r="J6" t="s">
-        <v>128</v>
-      </c>
-      <c r="K6" t="s">
-        <v>133</v>
-      </c>
-      <c r="L6" t="s">
-        <v>133</v>
-      </c>
-      <c r="M6" t="s">
-        <v>140</v>
-      </c>
-      <c r="X6">
-        <v>161.3</v>
-      </c>
-      <c r="Y6">
-        <v>74.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:83">
-      <c r="A7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" t="s">
-        <v>121</v>
-      </c>
-      <c r="I7" t="s">
-        <v>124</v>
-      </c>
-      <c r="J7" t="s">
-        <v>129</v>
-      </c>
-      <c r="K7" t="s">
-        <v>134</v>
-      </c>
-      <c r="L7" t="s">
-        <v>132</v>
-      </c>
-      <c r="M7" t="s">
-        <v>141</v>
-      </c>
-      <c r="N7">
-        <v>14.9</v>
-      </c>
-      <c r="O7">
-        <v>14.5</v>
-      </c>
-      <c r="P7">
-        <v>2182.8</v>
-      </c>
-      <c r="Q7">
-        <v>2279.4</v>
-      </c>
-      <c r="V7">
-        <v>50.3</v>
-      </c>
-      <c r="X7">
-        <v>231.3</v>
-      </c>
-      <c r="Y7">
-        <v>31.6</v>
-      </c>
-      <c r="Z7">
-        <v>3.69</v>
-      </c>
-      <c r="AA7">
-        <v>0.38</v>
-      </c>
-      <c r="AD7">
-        <v>22.6</v>
-      </c>
-      <c r="AE7">
-        <v>19.4</v>
-      </c>
-      <c r="AF7">
-        <v>12.6</v>
-      </c>
-      <c r="AG7">
-        <v>10.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:83">
-      <c r="A8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G8" t="s">
-        <v>117</v>
-      </c>
-      <c r="H8" t="s">
-        <v>123</v>
-      </c>
-      <c r="I8" t="s">
-        <v>124</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="F24" t="s">
         <v>130</v>
       </c>
-      <c r="K8" t="s">
-        <v>132</v>
-      </c>
-      <c r="L8" t="s">
-        <v>135</v>
-      </c>
-      <c r="M8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH8">
-        <v>63.7</v>
-      </c>
-      <c r="AI8">
-        <v>0.101</v>
-      </c>
-      <c r="AJ8">
-        <v>0.076</v>
-      </c>
-      <c r="AK8">
-        <v>0.068</v>
-      </c>
-      <c r="AL8">
-        <v>0.124</v>
-      </c>
-      <c r="AM8">
-        <v>0.056</v>
-      </c>
-      <c r="AN8">
-        <v>0.081</v>
-      </c>
-      <c r="AY8">
-        <v>6.78</v>
-      </c>
-      <c r="AZ8">
-        <v>0.468</v>
-      </c>
-      <c r="BA8">
-        <v>6.64</v>
-      </c>
-      <c r="BB8">
-        <v>0.061</v>
-      </c>
-      <c r="BC8">
-        <v>4.12</v>
-      </c>
-      <c r="BD8">
-        <v>0.654</v>
-      </c>
-      <c r="BF8">
-        <v>3.61</v>
-      </c>
-      <c r="BG8">
-        <v>63.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:83">
-      <c r="A9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H9" t="s">
-        <v>123</v>
-      </c>
-      <c r="I9" t="s">
-        <v>124</v>
-      </c>
-      <c r="J9" t="s">
-        <v>130</v>
-      </c>
-      <c r="K9" t="s">
-        <v>133</v>
-      </c>
-      <c r="L9" t="s">
-        <v>131</v>
-      </c>
-      <c r="M9" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH9">
-        <v>81.8</v>
-      </c>
-      <c r="AI9">
-        <v>0.227</v>
-      </c>
-      <c r="AJ9">
-        <v>0.186</v>
-      </c>
-      <c r="AK9">
-        <v>0.621</v>
-      </c>
-      <c r="AL9">
-        <v>0.424</v>
-      </c>
-      <c r="AM9">
-        <v>0.194</v>
-      </c>
-      <c r="AN9">
-        <v>0.247</v>
-      </c>
-      <c r="AO9">
-        <v>5.59</v>
-      </c>
-      <c r="AP9">
-        <v>0.576</v>
-      </c>
-      <c r="AQ9">
-        <v>7.13</v>
-      </c>
-      <c r="AR9">
-        <v>0.531</v>
-      </c>
-      <c r="AS9">
-        <v>8.039999999999999</v>
-      </c>
-      <c r="AT9">
-        <v>0.5620000000000001</v>
-      </c>
-      <c r="AU9">
-        <v>7.76</v>
-      </c>
-      <c r="AV9">
-        <v>0.569</v>
-      </c>
-      <c r="AW9">
-        <v>5.19</v>
-      </c>
-      <c r="AX9">
-        <v>5.59</v>
-      </c>
-      <c r="AY9">
-        <v>8.039999999999999</v>
-      </c>
-      <c r="AZ9">
-        <v>0.58</v>
-      </c>
-      <c r="BA9">
-        <v>7.76</v>
-      </c>
-      <c r="BB9">
-        <v>0.573</v>
-      </c>
-      <c r="BD9">
-        <v>0.136</v>
-      </c>
-      <c r="BE9">
-        <v>1.3</v>
-      </c>
-      <c r="BF9">
-        <v>5.19</v>
-      </c>
-      <c r="BG9">
-        <v>81.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:83">
-      <c r="A10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F10" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" t="s">
-        <v>119</v>
-      </c>
-      <c r="H10" t="s">
-        <v>121</v>
-      </c>
-      <c r="I10" t="s">
-        <v>124</v>
-      </c>
-      <c r="J10" t="s">
-        <v>127</v>
-      </c>
-      <c r="K10" t="s">
-        <v>131</v>
-      </c>
-      <c r="L10" t="s">
-        <v>134</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="G24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H24" t="s">
         <v>143</v>
       </c>
-      <c r="N10">
-        <v>22.6</v>
-      </c>
-      <c r="O10">
-        <v>24.9</v>
-      </c>
-      <c r="P10">
-        <v>1056.8</v>
-      </c>
-      <c r="Q10">
-        <v>1063.9</v>
-      </c>
-      <c r="R10">
-        <v>56.1</v>
-      </c>
-      <c r="S10">
-        <v>65.2</v>
-      </c>
-      <c r="U10">
-        <v>18.8</v>
-      </c>
-      <c r="V10">
-        <v>279.7</v>
-      </c>
-      <c r="W10">
-        <v>160.4</v>
-      </c>
-      <c r="X10">
-        <v>252.3</v>
-      </c>
-      <c r="Y10">
-        <v>17.3</v>
-      </c>
-      <c r="Z10">
-        <v>1.92</v>
-      </c>
-      <c r="AA10">
-        <v>0.649</v>
-      </c>
-      <c r="AB10">
-        <v>11.9</v>
-      </c>
-      <c r="AC10">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:83">
-      <c r="A11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" t="s">
-        <v>113</v>
-      </c>
-      <c r="G11" t="s">
-        <v>118</v>
-      </c>
-      <c r="H11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I11" t="s">
-        <v>124</v>
-      </c>
-      <c r="J11" t="s">
-        <v>130</v>
-      </c>
-      <c r="K11" t="s">
-        <v>131</v>
-      </c>
-      <c r="L11" t="s">
-        <v>131</v>
-      </c>
-      <c r="M11" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH11">
+      <c r="I24" t="s">
+        <v>144</v>
+      </c>
+      <c r="J24" t="s">
+        <v>153</v>
+      </c>
+      <c r="K24" t="s">
+        <v>154</v>
+      </c>
+      <c r="L24" t="s">
+        <v>154</v>
+      </c>
+      <c r="M24" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK24">
         <v>78.90000000000001</v>
       </c>
-      <c r="AI11">
+      <c r="AL24">
         <v>0.161</v>
       </c>
-      <c r="AJ11">
+      <c r="AM24">
         <v>0.291</v>
       </c>
-      <c r="AK11">
+      <c r="AN24">
         <v>0.514</v>
       </c>
-      <c r="AL11">
+      <c r="AO24">
         <v>0.47</v>
       </c>
-      <c r="AM11">
+      <c r="AP24">
         <v>0.066</v>
       </c>
-      <c r="AN11">
+      <c r="AQ24">
         <v>0.305</v>
       </c>
-      <c r="AO11">
+      <c r="AR24">
         <v>5.32</v>
       </c>
-      <c r="AP11">
+      <c r="AS24">
         <v>0.656</v>
       </c>
-      <c r="AQ11">
+      <c r="AT24">
         <v>6.85</v>
       </c>
-      <c r="AR11">
+      <c r="AU24">
         <v>0.572</v>
       </c>
-      <c r="AS11">
+      <c r="AV24">
         <v>7.85</v>
       </c>
-      <c r="AT11">
+      <c r="AW24">
         <v>0.591</v>
       </c>
-      <c r="AU11">
+      <c r="AX24">
         <v>7.43</v>
       </c>
-      <c r="AV11">
+      <c r="AY24">
         <v>0.589</v>
       </c>
-      <c r="AW11">
+      <c r="AZ24">
         <v>4.76</v>
       </c>
-      <c r="AX11">
+      <c r="BA24">
         <v>5.32</v>
       </c>
-      <c r="AY11">
+      <c r="BB24">
         <v>7.85</v>
       </c>
-      <c r="AZ11">
+      <c r="BC24">
         <v>0.608</v>
       </c>
-      <c r="BA11">
+      <c r="BD24">
         <v>7.43</v>
       </c>
-      <c r="BB11">
+      <c r="BE24">
         <v>0.589</v>
       </c>
-      <c r="BD11">
+      <c r="BG24">
         <v>0.173</v>
       </c>
-      <c r="BE11">
+      <c r="BH24">
         <v>0.173</v>
       </c>
-      <c r="BF11">
+      <c r="BI24">
         <v>4.65</v>
       </c>
-      <c r="BG11">
+      <c r="BJ24">
         <v>78.90000000000001</v>
       </c>
     </row>
@@ -2056,7 +3294,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2068,186 +3306,282 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="B12" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="B13" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>196</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>202</v>
+      </c>
+      <c r="B29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>204</v>
+      </c>
+      <c r="B31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>206</v>
+      </c>
+      <c r="B33" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>208</v>
+      </c>
+      <c r="B35" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>